<commit_message>
Cambios para correcto funcionamiento
</commit_message>
<xml_diff>
--- a/src/main/resources/MEDICIONES BERLANGA-ANDALUZ DEL 18 AL 21 DE ABRIL.xlsx
+++ b/src/main/resources/MEDICIONES BERLANGA-ANDALUZ DEL 18 AL 21 DE ABRIL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\JUAN\MIS DOCUMENTOS\IBERDROLA\2023\1.BURGOS-ARANDA-SORIA\4.MEDICIONES PARTES\ARANDA-SORIA\BERLANGA-ANDALUZ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\INES\Desktop\ROBERTO\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A87AFE0F-65A1-4F42-98E7-A8101A03C28D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D044F76-2DA0-44AF-95A9-32A812232978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C66C163A-FC94-45BE-AEE2-81A12E3FD87B}"/>
+    <workbookView xWindow="31665" yWindow="1440" windowWidth="21600" windowHeight="11370" xr2:uid="{C66C163A-FC94-45BE-AEE2-81A12E3FD87B}"/>
   </bookViews>
   <sheets>
     <sheet name="linea" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
   <si>
     <t>DÍA</t>
   </si>
@@ -154,6 +154,15 @@
   </si>
   <si>
     <t>SERGIO</t>
+  </si>
+  <si>
+    <t>PRUEBAS</t>
+  </si>
+  <si>
+    <t>SADÑLNSA</t>
+  </si>
+  <si>
+    <t>GAM</t>
   </si>
 </sst>
 </file>
@@ -645,84 +654,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -781,6 +712,84 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1103,7 +1112,7 @@
   <dimension ref="B1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1120,379 +1129,421 @@
   <sheetData>
     <row r="1" spans="2:12" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="35"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="46"/>
     </row>
     <row r="3" spans="2:12" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:12" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="49" t="s">
+      <c r="D4" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="50" t="s">
+      <c r="E4" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="50" t="s">
+      <c r="F4" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="50" t="s">
+      <c r="G4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="50" t="s">
+      <c r="H4" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="50" t="s">
+      <c r="I4" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="K4" s="52" t="s">
+      <c r="J4" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="K4" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="52" t="s">
+      <c r="L4" s="26" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="59">
+      <c r="B5" s="33">
         <v>33</v>
       </c>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60">
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34">
         <v>1</v>
       </c>
-      <c r="G5" s="60"/>
-      <c r="H5" s="60"/>
-      <c r="I5" s="60"/>
-      <c r="J5" s="61">
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="35">
         <v>45037</v>
       </c>
-      <c r="K5" s="62" t="s">
+      <c r="K5" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="L5" s="63"/>
+      <c r="L5" s="37"/>
     </row>
     <row r="6" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="64">
+      <c r="B6" s="38">
         <v>38</v>
       </c>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56">
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30">
         <v>1</v>
       </c>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="56"/>
-      <c r="J6" s="57">
+      <c r="G6" s="30"/>
+      <c r="H6" s="30">
+        <v>76</v>
+      </c>
+      <c r="I6" s="30"/>
+      <c r="J6" s="31">
         <v>45037</v>
       </c>
-      <c r="K6" s="58" t="s">
+      <c r="K6" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="L6" s="65"/>
+      <c r="L6" s="39" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="7" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="64">
+      <c r="B7" s="38">
         <v>39</v>
       </c>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56">
+      <c r="C7" s="30">
+        <v>34</v>
+      </c>
+      <c r="D7" s="30">
+        <v>34</v>
+      </c>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30">
         <v>1</v>
       </c>
-      <c r="G7" s="56"/>
-      <c r="H7" s="56"/>
-      <c r="I7" s="56"/>
-      <c r="J7" s="57">
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30">
+        <v>10</v>
+      </c>
+      <c r="J7" s="31">
         <v>45037</v>
       </c>
-      <c r="K7" s="58" t="s">
+      <c r="K7" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="L7" s="65"/>
+      <c r="L7" s="39"/>
     </row>
     <row r="8" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="64">
+      <c r="B8" s="38">
         <v>127</v>
       </c>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56">
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30">
         <v>1</v>
       </c>
-      <c r="G8" s="56"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="56"/>
-      <c r="J8" s="57">
+      <c r="G8" s="30"/>
+      <c r="H8" s="30">
+        <v>434</v>
+      </c>
+      <c r="I8" s="30"/>
+      <c r="J8" s="31">
         <v>45037</v>
       </c>
-      <c r="K8" s="58" t="s">
+      <c r="K8" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="L8" s="65"/>
+      <c r="L8" s="39"/>
     </row>
     <row r="9" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="64">
+      <c r="B9" s="38">
         <v>214</v>
       </c>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="56">
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30">
+        <v>43434</v>
+      </c>
+      <c r="F9" s="30">
         <v>1</v>
       </c>
-      <c r="G9" s="56"/>
-      <c r="H9" s="56"/>
-      <c r="I9" s="56"/>
-      <c r="J9" s="57">
+      <c r="G9" s="30">
+        <v>434</v>
+      </c>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="31">
         <v>44671</v>
       </c>
-      <c r="K9" s="58" t="s">
+      <c r="K9" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="L9" s="65"/>
+      <c r="L9" s="39"/>
     </row>
     <row r="10" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="64">
+      <c r="B10" s="38">
         <v>207</v>
       </c>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56">
+      <c r="C10" s="30">
+        <v>45</v>
+      </c>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30">
+        <v>565</v>
+      </c>
+      <c r="F10" s="30">
         <v>1</v>
       </c>
-      <c r="G10" s="56"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="57">
+      <c r="G10" s="30"/>
+      <c r="H10" s="30">
+        <v>434</v>
+      </c>
+      <c r="I10" s="30"/>
+      <c r="J10" s="31">
         <v>44671</v>
       </c>
-      <c r="K10" s="58" t="s">
+      <c r="K10" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="L10" s="65"/>
+      <c r="L10" s="39"/>
     </row>
     <row r="11" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="64">
+      <c r="B11" s="38">
         <v>193</v>
       </c>
-      <c r="C11" s="56"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="56">
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30">
         <v>1</v>
       </c>
-      <c r="G11" s="56"/>
-      <c r="H11" s="56"/>
-      <c r="I11" s="56"/>
-      <c r="J11" s="57">
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="31">
         <v>44671</v>
       </c>
-      <c r="K11" s="58" t="s">
+      <c r="K11" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="L11" s="65"/>
+      <c r="L11" s="39" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="12" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="64">
+      <c r="B12" s="38">
         <v>194</v>
       </c>
-      <c r="C12" s="56"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56">
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30">
         <v>1</v>
       </c>
-      <c r="G12" s="56"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="56"/>
-      <c r="J12" s="57">
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30">
+        <v>20</v>
+      </c>
+      <c r="J12" s="31">
         <v>44671</v>
       </c>
-      <c r="K12" s="58" t="s">
+      <c r="K12" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="L12" s="65"/>
+      <c r="L12" s="39"/>
     </row>
     <row r="13" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="64">
+      <c r="B13" s="38">
         <v>159</v>
       </c>
-      <c r="C13" s="56"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="56">
+      <c r="C13" s="30">
+        <v>4343</v>
+      </c>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30">
         <v>1</v>
       </c>
-      <c r="G13" s="56"/>
-      <c r="H13" s="56"/>
-      <c r="I13" s="56"/>
-      <c r="J13" s="57">
+      <c r="G13" s="30">
+        <v>434</v>
+      </c>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="31">
         <v>44671</v>
       </c>
-      <c r="K13" s="58" t="s">
+      <c r="K13" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="L13" s="65"/>
+      <c r="L13" s="39"/>
     </row>
     <row r="14" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="64">
+      <c r="B14" s="38">
         <v>158</v>
       </c>
-      <c r="C14" s="56"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56">
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30">
         <v>1</v>
       </c>
-      <c r="G14" s="56"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="57">
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="31">
         <v>44671</v>
       </c>
-      <c r="K14" s="58" t="s">
+      <c r="K14" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="L14" s="65"/>
+      <c r="L14" s="39" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="15" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="64">
+      <c r="B15" s="38">
         <v>163</v>
       </c>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56">
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30">
+        <v>777</v>
+      </c>
+      <c r="F15" s="30">
         <v>1</v>
       </c>
-      <c r="G15" s="56"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="57">
+      <c r="G15" s="30"/>
+      <c r="H15" s="30">
+        <v>434</v>
+      </c>
+      <c r="I15" s="30"/>
+      <c r="J15" s="31">
         <v>44671</v>
       </c>
-      <c r="K15" s="58" t="s">
+      <c r="K15" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="L15" s="65"/>
+      <c r="L15" s="39"/>
     </row>
     <row r="16" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="64">
+      <c r="B16" s="38">
         <v>247</v>
       </c>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56">
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30">
         <v>1</v>
       </c>
-      <c r="G16" s="56"/>
-      <c r="H16" s="56"/>
-      <c r="I16" s="56"/>
-      <c r="J16" s="57">
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="31">
         <v>45034</v>
       </c>
-      <c r="K16" s="58" t="s">
+      <c r="K16" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="L16" s="65"/>
+      <c r="L16" s="39"/>
     </row>
     <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="64">
+      <c r="B17" s="38">
         <v>243</v>
       </c>
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="56">
+      <c r="C17" s="30"/>
+      <c r="D17" s="30">
+        <v>43</v>
+      </c>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30">
         <v>1</v>
       </c>
-      <c r="G17" s="56"/>
-      <c r="H17" s="56"/>
-      <c r="I17" s="56"/>
-      <c r="J17" s="57">
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30">
+        <v>3</v>
+      </c>
+      <c r="J17" s="31">
         <v>45034</v>
       </c>
-      <c r="K17" s="58" t="s">
+      <c r="K17" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="L17" s="65"/>
+      <c r="L17" s="39"/>
     </row>
     <row r="18" spans="2:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="66">
+      <c r="B18" s="40">
         <v>240</v>
       </c>
-      <c r="C18" s="67"/>
-      <c r="D18" s="67"/>
-      <c r="E18" s="67"/>
-      <c r="F18" s="67">
+      <c r="C18" s="41"/>
+      <c r="D18" s="41">
+        <v>24</v>
+      </c>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41">
         <v>1</v>
       </c>
-      <c r="G18" s="67"/>
-      <c r="H18" s="67"/>
-      <c r="I18" s="67"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
       <c r="J18" s="12">
         <v>45034</v>
       </c>
-      <c r="K18" s="68" t="s">
+      <c r="K18" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="L18" s="69"/>
+      <c r="L18" s="43"/>
     </row>
     <row r="19" spans="2:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="53" t="s">
+      <c r="B19" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="54">
+      <c r="C19" s="28">
         <f>SUM(C5:C5)</f>
         <v>0</v>
       </c>
-      <c r="D19" s="54">
+      <c r="D19" s="28">
         <f>SUM(D5:D5)</f>
         <v>0</v>
       </c>
-      <c r="E19" s="54">
+      <c r="E19" s="28">
         <f>SUM(E5:E5)</f>
         <v>0</v>
       </c>
-      <c r="F19" s="54">
+      <c r="F19" s="28">
         <f>SUM(F5:F18)</f>
         <v>14</v>
       </c>
-      <c r="G19" s="54">
+      <c r="G19" s="28">
         <f>SUM(G5:G5)</f>
         <v>0</v>
       </c>
-      <c r="H19" s="54">
+      <c r="H19" s="28">
         <f>SUM(H5:H5)</f>
         <v>0</v>
       </c>
-      <c r="I19" s="55">
+      <c r="I19" s="29">
         <f>SUM(I5:I5)</f>
         <v>0</v>
       </c>
@@ -1522,13 +1573,13 @@
       <c r="I20" s="21"/>
     </row>
     <row r="23" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="36"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="47"/>
       <c r="I23" s="13"/>
     </row>
     <row r="24" spans="2:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1536,10 +1587,10 @@
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="7"/>
-      <c r="F24" s="42" t="s">
+      <c r="F24" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="G24" s="43"/>
+      <c r="G24" s="54"/>
       <c r="H24" s="5" t="s">
         <v>7</v>
       </c>
@@ -1549,17 +1600,17 @@
       </c>
     </row>
     <row r="25" spans="2:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="39" t="s">
+      <c r="B25" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="44">
+      <c r="C25" s="51"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="52"/>
+      <c r="F25" s="55">
         <f>C20</f>
         <v>0</v>
       </c>
-      <c r="G25" s="45"/>
+      <c r="G25" s="56"/>
       <c r="H25" s="1">
         <v>4600</v>
       </c>
@@ -1570,17 +1621,17 @@
       </c>
     </row>
     <row r="26" spans="2:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="39" t="s">
+      <c r="B26" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="44">
+      <c r="C26" s="51"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="52"/>
+      <c r="F26" s="55">
         <f>D20</f>
         <v>0</v>
       </c>
-      <c r="G26" s="45"/>
+      <c r="G26" s="56"/>
       <c r="H26" s="1">
         <v>1200</v>
       </c>
@@ -1591,17 +1642,17 @@
       </c>
     </row>
     <row r="27" spans="2:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="39" t="s">
+      <c r="B27" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="40"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="44">
+      <c r="C27" s="51"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="52"/>
+      <c r="F27" s="55">
         <f>E20</f>
         <v>0</v>
       </c>
-      <c r="G27" s="45"/>
+      <c r="G27" s="56"/>
       <c r="H27" s="1">
         <v>9200</v>
       </c>
@@ -1612,17 +1663,17 @@
       </c>
     </row>
     <row r="28" spans="2:12" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="47" t="s">
+      <c r="B28" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="47"/>
-      <c r="D28" s="47"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="46">
+      <c r="C28" s="58"/>
+      <c r="D28" s="58"/>
+      <c r="E28" s="58"/>
+      <c r="F28" s="57">
         <f>H20</f>
         <v>0</v>
       </c>
-      <c r="G28" s="46"/>
+      <c r="G28" s="57"/>
       <c r="H28" s="2">
         <v>2500</v>
       </c>
@@ -1633,15 +1684,15 @@
       </c>
     </row>
     <row r="29" spans="2:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="37" t="s">
+      <c r="B29" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="49"/>
       <c r="I29" s="14"/>
       <c r="J29" s="3">
         <f>SUM(J25:J28)</f>
@@ -1681,17 +1732,17 @@
       </c>
     </row>
     <row r="33" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="25" t="s">
+      <c r="B33" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="22">
+      <c r="C33" s="62"/>
+      <c r="D33" s="62"/>
+      <c r="E33" s="62"/>
+      <c r="F33" s="59">
         <f>F19</f>
         <v>14</v>
       </c>
-      <c r="G33" s="22"/>
+      <c r="G33" s="59"/>
       <c r="H33" s="1">
         <v>250</v>
       </c>
@@ -1702,17 +1753,17 @@
       </c>
     </row>
     <row r="34" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="26" t="s">
+      <c r="B34" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="29">
+      <c r="C34" s="64"/>
+      <c r="D34" s="64"/>
+      <c r="E34" s="65"/>
+      <c r="F34" s="66">
         <f>G19</f>
         <v>0</v>
       </c>
-      <c r="G34" s="30"/>
+      <c r="G34" s="67"/>
       <c r="H34" s="1">
         <v>24</v>
       </c>
@@ -1723,17 +1774,17 @@
       </c>
     </row>
     <row r="35" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="26" t="s">
+      <c r="B35" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="28"/>
-      <c r="F35" s="29">
+      <c r="C35" s="64"/>
+      <c r="D35" s="64"/>
+      <c r="E35" s="65"/>
+      <c r="F35" s="66">
         <f>I19</f>
         <v>0</v>
       </c>
-      <c r="G35" s="31"/>
+      <c r="G35" s="68"/>
       <c r="H35" s="1">
         <v>50</v>
       </c>
@@ -1744,16 +1795,16 @@
       </c>
     </row>
     <row r="36" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="25" t="s">
+      <c r="B36" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="22">
-        <v>0</v>
-      </c>
-      <c r="G36" s="22"/>
+      <c r="C36" s="62"/>
+      <c r="D36" s="62"/>
+      <c r="E36" s="62"/>
+      <c r="F36" s="59">
+        <v>0</v>
+      </c>
+      <c r="G36" s="59"/>
       <c r="H36" s="1">
         <v>90</v>
       </c>
@@ -1764,16 +1815,16 @@
       </c>
     </row>
     <row r="37" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="25" t="s">
+      <c r="B37" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="22">
-        <v>0</v>
-      </c>
-      <c r="G37" s="22"/>
+      <c r="C37" s="62"/>
+      <c r="D37" s="62"/>
+      <c r="E37" s="62"/>
+      <c r="F37" s="59">
+        <v>0</v>
+      </c>
+      <c r="G37" s="59"/>
       <c r="H37" s="1">
         <v>240.45</v>
       </c>
@@ -1785,14 +1836,14 @@
       <c r="L37" s="17"/>
     </row>
     <row r="38" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="25" t="s">
+      <c r="B38" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
+      <c r="C38" s="62"/>
+      <c r="D38" s="62"/>
+      <c r="E38" s="62"/>
+      <c r="F38" s="59"/>
+      <c r="G38" s="59"/>
       <c r="H38" s="1">
         <v>10</v>
       </c>
@@ -1804,18 +1855,18 @@
       <c r="L38" s="17"/>
     </row>
     <row r="39" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="25" t="s">
+      <c r="B39" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="32" t="s">
+      <c r="C39" s="62"/>
+      <c r="D39" s="62"/>
+      <c r="E39" s="62"/>
+      <c r="F39" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="G39" s="32"/>
-      <c r="H39" s="32"/>
-      <c r="I39" s="32"/>
+      <c r="G39" s="69"/>
+      <c r="H39" s="69"/>
+      <c r="I39" s="69"/>
       <c r="J39" s="1"/>
       <c r="L39" s="17"/>
     </row>
@@ -1823,10 +1874,10 @@
       <c r="L40" s="17"/>
     </row>
     <row r="41" spans="2:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G41" s="23" t="s">
+      <c r="G41" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="H41" s="24"/>
+      <c r="H41" s="61"/>
       <c r="I41" s="16"/>
       <c r="J41" s="3">
         <f>J31+J33+J36+J37+J34+J35+J38+J39</f>
@@ -1842,18 +1893,6 @@
     <sortCondition ref="B5"/>
   </sortState>
   <mergeCells count="27">
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="B28:E28"/>
     <mergeCell ref="F33:G33"/>
     <mergeCell ref="G41:H41"/>
     <mergeCell ref="B36:E36"/>
@@ -1869,6 +1908,18 @@
     <mergeCell ref="B38:E38"/>
     <mergeCell ref="F38:G38"/>
     <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="B28:E28"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.55118110236220474" bottom="0.55118110236220474" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Num días totales trabajado funcionando corréctamente
</commit_message>
<xml_diff>
--- a/src/main/resources/MEDICIONES BERLANGA-ANDALUZ DEL 18 AL 21 DE ABRIL.xlsx
+++ b/src/main/resources/MEDICIONES BERLANGA-ANDALUZ DEL 18 AL 21 DE ABRIL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\INES\Desktop\ROBERTO\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D044F76-2DA0-44AF-95A9-32A812232978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703C20B5-7C90-41E3-8214-488BFE03511D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31665" yWindow="1440" windowWidth="21600" windowHeight="11370" xr2:uid="{C66C163A-FC94-45BE-AEE2-81A12E3FD87B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C66C163A-FC94-45BE-AEE2-81A12E3FD87B}"/>
   </bookViews>
   <sheets>
     <sheet name="linea" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>DÍA</t>
   </si>
@@ -163,6 +163,12 @@
   </si>
   <si>
     <t>GAM</t>
+  </si>
+  <si>
+    <t>PEPE</t>
+  </si>
+  <si>
+    <t>DAVID</t>
   </si>
 </sst>
 </file>
@@ -714,6 +720,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -758,39 +797,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1112,7 +1118,7 @@
   <dimension ref="B1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,19 +1135,19 @@
   <sheetData>
     <row r="1" spans="2:12" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="46"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="57"/>
     </row>
     <row r="3" spans="2:12" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:12" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1196,7 +1202,7 @@
         <v>45037</v>
       </c>
       <c r="K5" s="36" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="L5" s="37"/>
     </row>
@@ -1344,7 +1350,7 @@
         <v>44671</v>
       </c>
       <c r="K11" s="32" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="L11" s="39" t="s">
         <v>36</v>
@@ -1369,7 +1375,7 @@
         <v>44671</v>
       </c>
       <c r="K12" s="32" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="L12" s="39"/>
     </row>
@@ -1573,13 +1579,13 @@
       <c r="I20" s="21"/>
     </row>
     <row r="23" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="47"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="47"/>
+      <c r="B23" s="58"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="58"/>
+      <c r="G23" s="58"/>
+      <c r="H23" s="58"/>
       <c r="I23" s="13"/>
     </row>
     <row r="24" spans="2:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1587,10 +1593,10 @@
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="7"/>
-      <c r="F24" s="53" t="s">
+      <c r="F24" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="G24" s="54"/>
+      <c r="G24" s="65"/>
       <c r="H24" s="5" t="s">
         <v>7</v>
       </c>
@@ -1600,17 +1606,17 @@
       </c>
     </row>
     <row r="25" spans="2:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="50" t="s">
+      <c r="B25" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="51"/>
-      <c r="D25" s="51"/>
-      <c r="E25" s="52"/>
-      <c r="F25" s="55">
+      <c r="C25" s="62"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="63"/>
+      <c r="F25" s="66">
         <f>C20</f>
         <v>0</v>
       </c>
-      <c r="G25" s="56"/>
+      <c r="G25" s="67"/>
       <c r="H25" s="1">
         <v>4600</v>
       </c>
@@ -1621,17 +1627,17 @@
       </c>
     </row>
     <row r="26" spans="2:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="50" t="s">
+      <c r="B26" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="51"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="52"/>
-      <c r="F26" s="55">
+      <c r="C26" s="62"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="66">
         <f>D20</f>
         <v>0</v>
       </c>
-      <c r="G26" s="56"/>
+      <c r="G26" s="67"/>
       <c r="H26" s="1">
         <v>1200</v>
       </c>
@@ -1642,17 +1648,17 @@
       </c>
     </row>
     <row r="27" spans="2:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="50" t="s">
+      <c r="B27" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="51"/>
-      <c r="D27" s="51"/>
-      <c r="E27" s="52"/>
-      <c r="F27" s="55">
+      <c r="C27" s="62"/>
+      <c r="D27" s="62"/>
+      <c r="E27" s="63"/>
+      <c r="F27" s="66">
         <f>E20</f>
         <v>0</v>
       </c>
-      <c r="G27" s="56"/>
+      <c r="G27" s="67"/>
       <c r="H27" s="1">
         <v>9200</v>
       </c>
@@ -1663,17 +1669,17 @@
       </c>
     </row>
     <row r="28" spans="2:12" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="58" t="s">
+      <c r="B28" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="58"/>
-      <c r="D28" s="58"/>
-      <c r="E28" s="58"/>
-      <c r="F28" s="57">
+      <c r="C28" s="69"/>
+      <c r="D28" s="69"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="68">
         <f>H20</f>
         <v>0</v>
       </c>
-      <c r="G28" s="57"/>
+      <c r="G28" s="68"/>
       <c r="H28" s="2">
         <v>2500</v>
       </c>
@@ -1684,15 +1690,15 @@
       </c>
     </row>
     <row r="29" spans="2:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="48" t="s">
+      <c r="B29" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="49"/>
-      <c r="D29" s="49"/>
-      <c r="E29" s="49"/>
-      <c r="F29" s="49"/>
-      <c r="G29" s="49"/>
-      <c r="H29" s="49"/>
+      <c r="C29" s="60"/>
+      <c r="D29" s="60"/>
+      <c r="E29" s="60"/>
+      <c r="F29" s="60"/>
+      <c r="G29" s="60"/>
+      <c r="H29" s="60"/>
       <c r="I29" s="14"/>
       <c r="J29" s="3">
         <f>SUM(J25:J28)</f>
@@ -1732,17 +1738,17 @@
       </c>
     </row>
     <row r="33" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="62" t="s">
+      <c r="B33" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="62"/>
-      <c r="D33" s="62"/>
-      <c r="E33" s="62"/>
-      <c r="F33" s="59">
+      <c r="C33" s="47"/>
+      <c r="D33" s="47"/>
+      <c r="E33" s="47"/>
+      <c r="F33" s="44">
         <f>F19</f>
         <v>14</v>
       </c>
-      <c r="G33" s="59"/>
+      <c r="G33" s="44"/>
       <c r="H33" s="1">
         <v>250</v>
       </c>
@@ -1753,17 +1759,17 @@
       </c>
     </row>
     <row r="34" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="63" t="s">
+      <c r="B34" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="64"/>
-      <c r="D34" s="64"/>
-      <c r="E34" s="65"/>
-      <c r="F34" s="66">
+      <c r="C34" s="49"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="51">
         <f>G19</f>
         <v>0</v>
       </c>
-      <c r="G34" s="67"/>
+      <c r="G34" s="52"/>
       <c r="H34" s="1">
         <v>24</v>
       </c>
@@ -1774,17 +1780,17 @@
       </c>
     </row>
     <row r="35" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="63" t="s">
+      <c r="B35" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="C35" s="64"/>
-      <c r="D35" s="64"/>
-      <c r="E35" s="65"/>
-      <c r="F35" s="66">
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="51">
         <f>I19</f>
         <v>0</v>
       </c>
-      <c r="G35" s="68"/>
+      <c r="G35" s="53"/>
       <c r="H35" s="1">
         <v>50</v>
       </c>
@@ -1795,16 +1801,16 @@
       </c>
     </row>
     <row r="36" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="62" t="s">
+      <c r="B36" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="62"/>
-      <c r="D36" s="62"/>
-      <c r="E36" s="62"/>
-      <c r="F36" s="59">
-        <v>0</v>
-      </c>
-      <c r="G36" s="59"/>
+      <c r="C36" s="47"/>
+      <c r="D36" s="47"/>
+      <c r="E36" s="47"/>
+      <c r="F36" s="44">
+        <v>0</v>
+      </c>
+      <c r="G36" s="44"/>
       <c r="H36" s="1">
         <v>90</v>
       </c>
@@ -1815,16 +1821,16 @@
       </c>
     </row>
     <row r="37" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="62" t="s">
+      <c r="B37" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="62"/>
-      <c r="D37" s="62"/>
-      <c r="E37" s="62"/>
-      <c r="F37" s="59">
-        <v>0</v>
-      </c>
-      <c r="G37" s="59"/>
+      <c r="C37" s="47"/>
+      <c r="D37" s="47"/>
+      <c r="E37" s="47"/>
+      <c r="F37" s="44">
+        <v>0</v>
+      </c>
+      <c r="G37" s="44"/>
       <c r="H37" s="1">
         <v>240.45</v>
       </c>
@@ -1836,14 +1842,14 @@
       <c r="L37" s="17"/>
     </row>
     <row r="38" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="62" t="s">
+      <c r="B38" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="C38" s="62"/>
-      <c r="D38" s="62"/>
-      <c r="E38" s="62"/>
-      <c r="F38" s="59"/>
-      <c r="G38" s="59"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="47"/>
+      <c r="F38" s="44"/>
+      <c r="G38" s="44"/>
       <c r="H38" s="1">
         <v>10</v>
       </c>
@@ -1855,18 +1861,18 @@
       <c r="L38" s="17"/>
     </row>
     <row r="39" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="62" t="s">
+      <c r="B39" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C39" s="62"/>
-      <c r="D39" s="62"/>
-      <c r="E39" s="62"/>
-      <c r="F39" s="69" t="s">
+      <c r="C39" s="47"/>
+      <c r="D39" s="47"/>
+      <c r="E39" s="47"/>
+      <c r="F39" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="G39" s="69"/>
-      <c r="H39" s="69"/>
-      <c r="I39" s="69"/>
+      <c r="G39" s="54"/>
+      <c r="H39" s="54"/>
+      <c r="I39" s="54"/>
       <c r="J39" s="1"/>
       <c r="L39" s="17"/>
     </row>
@@ -1874,10 +1880,10 @@
       <c r="L40" s="17"/>
     </row>
     <row r="41" spans="2:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G41" s="60" t="s">
+      <c r="G41" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="H41" s="61"/>
+      <c r="H41" s="46"/>
       <c r="I41" s="16"/>
       <c r="J41" s="3">
         <f>J31+J33+J36+J37+J34+J35+J38+J39</f>
@@ -1893,6 +1899,18 @@
     <sortCondition ref="B5"/>
   </sortState>
   <mergeCells count="27">
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="B28:E28"/>
     <mergeCell ref="F33:G33"/>
     <mergeCell ref="G41:H41"/>
     <mergeCell ref="B36:E36"/>
@@ -1908,18 +1926,6 @@
     <mergeCell ref="B38:E38"/>
     <mergeCell ref="F38:G38"/>
     <mergeCell ref="B33:E33"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="B28:E28"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.55118110236220474" bottom="0.55118110236220474" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Cambios en excels para pruebas
</commit_message>
<xml_diff>
--- a/src/main/resources/MEDICIONES BERLANGA-ANDALUZ DEL 18 AL 21 DE ABRIL.xlsx
+++ b/src/main/resources/MEDICIONES BERLANGA-ANDALUZ DEL 18 AL 21 DE ABRIL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\INES\Desktop\ROBERTO\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB6C03E-0C93-4A22-AD72-66629E47B779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DE561A-401A-4660-8402-8B3411BA156C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C66C163A-FC94-45BE-AEE2-81A12E3FD87B}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
   <si>
     <t>DÍA</t>
   </si>
@@ -156,19 +156,52 @@
     <t>SERGIO</t>
   </si>
   <si>
-    <t>PRUEBAS</t>
-  </si>
-  <si>
-    <t>SADÑLNSA</t>
-  </si>
-  <si>
-    <t>GAM</t>
-  </si>
-  <si>
     <t>PEPE</t>
   </si>
   <si>
     <t>DAVID</t>
+  </si>
+  <si>
+    <t>UNO</t>
+  </si>
+  <si>
+    <t>DOS</t>
+  </si>
+  <si>
+    <t>TRES</t>
+  </si>
+  <si>
+    <t>CUATRO</t>
+  </si>
+  <si>
+    <t>CINCO</t>
+  </si>
+  <si>
+    <t>SEIS</t>
+  </si>
+  <si>
+    <t>SIETE</t>
+  </si>
+  <si>
+    <t>OCHO</t>
+  </si>
+  <si>
+    <t>NUEVE</t>
+  </si>
+  <si>
+    <t>DIEZ</t>
+  </si>
+  <si>
+    <t>ONCE</t>
+  </si>
+  <si>
+    <t>DOCE</t>
+  </si>
+  <si>
+    <t>TRECE</t>
+  </si>
+  <si>
+    <t>CATORCE</t>
   </si>
 </sst>
 </file>
@@ -1118,7 +1151,7 @@
   <dimension ref="B1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1202,9 +1235,11 @@
         <v>45037</v>
       </c>
       <c r="K5" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="L5" s="37"/>
+        <v>35</v>
+      </c>
+      <c r="L5" s="37" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="6" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="38">
@@ -1228,7 +1263,7 @@
         <v>33</v>
       </c>
       <c r="L6" s="39" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1256,7 +1291,9 @@
       <c r="K7" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="L7" s="39"/>
+      <c r="L7" s="39" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="8" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="38">
@@ -1279,7 +1316,9 @@
       <c r="K8" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="L8" s="39"/>
+      <c r="L8" s="39" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="9" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="38">
@@ -1304,7 +1343,9 @@
       <c r="K9" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="L9" s="39"/>
+      <c r="L9" s="39" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="10" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="38">
@@ -1331,7 +1372,9 @@
       <c r="K10" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="L10" s="39"/>
+      <c r="L10" s="39" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="11" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="38">
@@ -1350,10 +1393,10 @@
         <v>44671</v>
       </c>
       <c r="K11" s="32" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="L11" s="39" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1375,9 +1418,11 @@
         <v>44671</v>
       </c>
       <c r="K12" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="L12" s="39"/>
+        <v>34</v>
+      </c>
+      <c r="L12" s="39" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="13" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="38">
@@ -1402,7 +1447,9 @@
       <c r="K13" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="L13" s="39"/>
+      <c r="L13" s="39" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="14" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="38">
@@ -1424,7 +1471,7 @@
         <v>33</v>
       </c>
       <c r="L14" s="39" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1450,7 +1497,9 @@
       <c r="K15" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="L15" s="39"/>
+      <c r="L15" s="39" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="16" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="38">
@@ -1471,7 +1520,9 @@
       <c r="K16" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="L16" s="39"/>
+      <c r="L16" s="39" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="38">
@@ -1496,7 +1547,9 @@
       <c r="K17" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="L17" s="39"/>
+      <c r="L17" s="39" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="18" spans="2:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="40">
@@ -1519,38 +1572,40 @@
       <c r="K18" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="L18" s="43"/>
+      <c r="L18" s="43" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="19" spans="2:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="27" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="28">
-        <f>SUM(C5:C18)</f>
+        <f t="shared" ref="C19:I19" si="0">SUM(C5:C18)</f>
         <v>4422</v>
       </c>
       <c r="D19" s="28">
-        <f>SUM(D5:D18)</f>
+        <f t="shared" si="0"/>
         <v>101</v>
       </c>
       <c r="E19" s="28">
-        <f>SUM(E5:E18)</f>
+        <f t="shared" si="0"/>
         <v>44776</v>
       </c>
       <c r="F19" s="28">
-        <f>SUM(F5:F18)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="G19" s="28">
-        <f>SUM(G5:G18)</f>
+        <f t="shared" si="0"/>
         <v>868</v>
       </c>
       <c r="H19" s="28">
-        <f>SUM(H5:H18)</f>
+        <f t="shared" si="0"/>
         <v>1378</v>
       </c>
       <c r="I19" s="29">
-        <f>SUM(I5:I18)</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
     </row>
@@ -1816,7 +1871,7 @@
       </c>
       <c r="I36" s="1"/>
       <c r="J36" s="1">
-        <f t="shared" ref="J36" si="0">F36*H36</f>
+        <f t="shared" ref="J36" si="1">F36*H36</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>